<commit_message>
Added functionality to rate existing distributor. Added getDistType(), findWithAttr(), and getFractionalSize() functions.
</commit_message>
<xml_diff>
--- a/site/data/distObjects.xlsx
+++ b/site/data/distObjects.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5728" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5732" uniqueCount="434">
   <si>
     <t>bodyStyle</t>
   </si>
@@ -1687,10 +1687,10 @@
   <dimension ref="A1:S493"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B104" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O137" sqref="O137:O493"/>
+      <selection pane="bottomRight" activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7552,6 +7552,9 @@
       <c r="A111" s="1" t="s">
         <v>430</v>
       </c>
+      <c r="B111" s="1">
+        <v>1605</v>
+      </c>
       <c r="C111" s="1" t="s">
         <v>27</v>
       </c>
@@ -7599,6 +7602,15 @@
       <c r="A112" s="1" t="s">
         <v>430</v>
       </c>
+      <c r="B112" s="1">
+        <v>1605</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="E112" s="8">
         <v>2</v>
       </c>
@@ -7639,6 +7651,15 @@
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>430</v>
+      </c>
+      <c r="B113" s="1">
+        <v>1605</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E113" s="8">
         <v>2</v>

</xml_diff>